<commit_message>
IN-1009 merge P1 remarks mapping spreadsheet with warnings spreadsheet
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FDF87E-0019-3B4A-9607-B81D9A3B9285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD30A45-11D3-9E4C-945C-61BE1854084C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30040" yWindow="6760" windowWidth="27680" windowHeight="18820" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7460" yWindow="9540" windowWidth="49560" windowHeight="23720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
     <sheet name="client_violent_warnings" sheetId="1" r:id="rId2"/>
-    <sheet name="deputy_violent_warnings" sheetId="2" r:id="rId3"/>
-    <sheet name="warning_violent_lookup" sheetId="3" r:id="rId4"/>
-    <sheet name="client_special_warnings" sheetId="4" r:id="rId5"/>
-    <sheet name="deputy_special_warnings" sheetId="5" r:id="rId6"/>
-    <sheet name="client_saarcheck_warnings" sheetId="6" r:id="rId7"/>
-    <sheet name="client_nodebtchase_warnings" sheetId="7" r:id="rId8"/>
-    <sheet name="person_warning" sheetId="8" r:id="rId9"/>
+    <sheet name="p1_client_remarks_warnings" sheetId="10" r:id="rId3"/>
+    <sheet name="p1_deputy_remarks_warnings" sheetId="11" r:id="rId4"/>
+    <sheet name="deputy_violent_warnings" sheetId="2" r:id="rId5"/>
+    <sheet name="warning_violent_lookup" sheetId="3" r:id="rId6"/>
+    <sheet name="client_special_warnings" sheetId="4" r:id="rId7"/>
+    <sheet name="deputy_special_warnings" sheetId="5" r:id="rId8"/>
+    <sheet name="client_saarcheck_warnings" sheetId="6" r:id="rId9"/>
+    <sheet name="client_nodebtchase_warnings" sheetId="7" r:id="rId10"/>
+    <sheet name="person_warning" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="108">
   <si>
     <t>table_name</t>
   </si>
@@ -321,6 +323,51 @@
   </si>
   <si>
     <t>Casrec Migration - No Debt to be chased</t>
+  </si>
+  <si>
+    <t>REMARKS</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Logdate</t>
+  </si>
+  <si>
+    <t>Confirm migration user from refinement</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>p1_client_remarks_warnings</t>
+  </si>
+  <si>
+    <t>p1_deputy_remarks_warnings</t>
+  </si>
+  <si>
+    <t>deputy_remarks</t>
+  </si>
+  <si>
+    <t>Pri = 1</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Pri, Case</t>
+  </si>
+  <si>
+    <t>Pri, Deputy No</t>
+  </si>
+  <si>
+    <t>DEPUTY_REMARKS</t>
+  </si>
+  <si>
+    <t>Log Date</t>
   </si>
 </sst>
 </file>
@@ -330,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -390,6 +437,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -432,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -462,6 +515,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,15 +899,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9D2251-14B4-1F49-81A1-F886FE8AA11B}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1021,20 +1080,523 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="18" t="s">
+      <c r="B10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:Z9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="11.5"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="74" customWidth="1"/>
+    <col min="7" max="7" width="11.5"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="73.5" customWidth="1"/>
+    <col min="18" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="6">
+        <v>2</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="P4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:Z3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="14" width="8.6640625" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15">
+      <c r="A3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -1042,10 +1604,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" sqref="A1:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1368,13 +1930,597 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF70CE53-3D87-3240-84FD-6CFC5D7D9F94}">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="6" max="6" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="M4" s="6"/>
+      <c r="P4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" ht="15">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="4"/>
+      <c r="M5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="15">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="15">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="1:17" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F41986-8AFC-D74D-A8C4-BEC2E0AB83ED}">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="6" max="6" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="M4" s="6"/>
+      <c r="P4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" ht="15">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="4"/>
+      <c r="M5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="15">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="15">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="1:17" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1698,7 +2844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
@@ -2006,14 +3152,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2338,11 +3484,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
@@ -2669,7 +3815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
@@ -2999,461 +4145,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Z9"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="11.5"/>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="74" customWidth="1"/>
-    <col min="7" max="7" width="11.5"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="22.5" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" customWidth="1"/>
-    <col min="15" max="15" width="18.33203125" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="73.5" customWidth="1"/>
-    <col min="18" max="1025" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="15">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-    </row>
-    <row r="2" spans="1:26" ht="15">
-      <c r="A2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="6">
-        <v>2</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="P4" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15">
-      <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:Z3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="14" width="8.6640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-    </row>
-    <row r="2" spans="1:26" ht="15">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15">
-      <c r="A3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Set assignees_id to migration user for warnings entity
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010CE1D2-0116-6B49-854F-62D97CF5D04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E5741A-4B42-DB49-9BB9-34934FF7E619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="6920" windowWidth="35400" windowHeight="21880" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="35400" windowHeight="19460" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="104">
   <si>
     <t>table_name</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Need a migration user for this possibly as we do not have any asignee ids for markers. This does not show in the front end either</t>
-  </si>
-  <si>
     <t>closed_by</t>
   </si>
   <si>
@@ -333,9 +330,6 @@
     <t>Logdate</t>
   </si>
   <si>
-    <t>Confirm migration user from refinement</t>
-  </si>
-  <si>
     <t>remarks</t>
   </si>
   <si>
@@ -351,9 +345,6 @@
     <t>Pri = 1</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -361,6 +352,9 @@
   </si>
   <si>
     <t>Pri, Deputy No</t>
+  </si>
+  <si>
+    <t>Set to migration user</t>
   </si>
 </sst>
 </file>
@@ -909,148 +903,148 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>73</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>76</v>
-      </c>
       <c r="H3" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>78</v>
-      </c>
       <c r="H4" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="H5" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>17</v>
@@ -1059,21 +1053,21 @@
         <v>17</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>17</v>
@@ -1082,53 +1076,53 @@
         <v>17</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G8" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>101</v>
-      </c>
       <c r="H9" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1222,13 +1216,13 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -1238,18 +1232,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15">
       <c r="A3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -1259,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1272,10 +1266,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1407,13 +1401,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>2</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -1424,7 +1418,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -1446,23 +1440,23 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1470,7 +1464,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -1481,23 +1475,23 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1505,7 +1499,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -1516,33 +1510,33 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -1553,10 +1547,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -1574,10 +1568,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>
@@ -1602,7 +1596,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1710,13 +1704,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>1</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15">
@@ -1727,7 +1721,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -1751,10 +1745,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E5" s="5" t="b">
         <f>FALSE()</f>
@@ -1764,12 +1758,12 @@
       <c r="J5" s="7"/>
       <c r="K5" s="4"/>
       <c r="M5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="9"/>
     </row>
@@ -1781,27 +1775,27 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="K6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="6"/>
     </row>
@@ -1813,27 +1807,27 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5"/>
       <c r="O7" s="4"/>
       <c r="P7" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
@@ -1845,10 +1839,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -1866,10 +1860,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>
@@ -1879,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1891,10 +1885,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2026,13 +2020,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>2</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -2043,7 +2037,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -2065,24 +2059,24 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2090,7 +2084,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -2101,23 +2095,23 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="7"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2125,7 +2119,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -2136,34 +2130,34 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -2174,10 +2168,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -2195,10 +2189,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>
@@ -2235,16 +2229,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15">
       <c r="A1" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -2275,10 +2269,10 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -2309,10 +2303,10 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="13"/>
@@ -2339,14 +2333,14 @@
     </row>
     <row r="4" spans="1:26" ht="15">
       <c r="A4" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="13"/>
@@ -2377,10 +2371,10 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="13"/>
@@ -2533,7 +2527,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2665,13 +2659,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>2</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -2682,7 +2676,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -2704,24 +2698,24 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2729,7 +2723,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -2740,24 +2734,24 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2765,7 +2759,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -2776,34 +2770,34 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -2814,10 +2808,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -2835,10 +2829,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>
@@ -2864,7 +2858,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2996,13 +2990,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>2</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -3013,7 +3007,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -3035,24 +3029,24 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -3060,7 +3054,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -3071,24 +3065,24 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3096,7 +3090,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -3107,34 +3101,34 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -3145,10 +3139,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -3166,10 +3160,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>
@@ -3193,10 +3187,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3328,13 +3322,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>2</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -3345,7 +3339,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -3367,24 +3361,24 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -3392,7 +3386,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -3403,24 +3397,24 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3428,7 +3422,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -3439,34 +3433,34 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -3477,10 +3471,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -3498,10 +3492,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>
@@ -3525,10 +3519,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3660,13 +3654,13 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>2</v>
+        <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -3677,7 +3671,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
@@ -3699,24 +3693,24 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -3724,7 +3718,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -3735,24 +3729,24 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3760,7 +3754,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -3771,34 +3765,34 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -3809,10 +3803,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="b">
         <f>FALSE()</f>
@@ -3830,10 +3824,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E9" s="5" t="b">
         <f>FALSE()</f>

</xml_diff>

<commit_message>
Remove deputy_p1_remarks from Warnings spreadsheet
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E5741A-4B42-DB49-9BB9-34934FF7E619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EFAEFA-1835-C043-AFD2-8B4CF28D9D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="35400" windowHeight="19460" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="35400" windowHeight="19460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="101">
   <si>
     <t>table_name</t>
   </si>
@@ -336,12 +336,6 @@
     <t>p1_client_remarks_warnings</t>
   </si>
   <si>
-    <t>p1_deputy_remarks_warnings</t>
-  </si>
-  <si>
-    <t>deputy_remarks</t>
-  </si>
-  <si>
     <t>Pri = 1</t>
   </si>
   <si>
@@ -349,9 +343,6 @@
   </si>
   <si>
     <t>Pri, Case</t>
-  </si>
-  <si>
-    <t>Pri, Deputy No</t>
   </si>
   <si>
     <t>Set to migration user</t>
@@ -886,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9D2251-14B4-1F49-81A1-F886FE8AA11B}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1082,46 +1073,23 @@
         <v>95</v>
       </c>
       <c r="G8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="18" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1404,10 +1372,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -1707,10 +1675,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15">
@@ -1763,7 +1731,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="9"/>
     </row>
@@ -1795,7 +1763,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q6" s="6"/>
     </row>
@@ -1827,7 +1795,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="4"/>
       <c r="P7" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
@@ -1873,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2023,10 +1991,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -2662,10 +2630,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -2993,10 +2961,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -3325,10 +3293,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">
@@ -3519,7 +3487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
@@ -3657,10 +3625,10 @@
         <v>2657</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15">

</xml_diff>

<commit_message>
Updates following pairing with Jack
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F471E059-E9F2-6449-9C1B-619B6455E888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E2BC4-31FE-8342-8452-9DB36BF6598B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -24,14 +24,12 @@
     <sheet name="client_nodebtchase_warnings" sheetId="7" r:id="rId9"/>
     <sheet name="person_warning" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -324,19 +322,19 @@
     <t>Deputy No, VWM</t>
   </si>
   <si>
-    <t>c_sim = not null</t>
-  </si>
-  <si>
-    <t>c_saar_check = not null</t>
-  </si>
-  <si>
-    <t>c_vwm = not null</t>
-  </si>
-  <si>
     <t>c_pri = 1</t>
   </si>
   <si>
-    <t>c_debt_chase = not null</t>
+    <t>include_values = {"col": "Debt chase", "values": ["1"]}</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "SAAR Check", "values": ["Y"]}</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "SIM", "values": ["3"]}</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "VWM", "values": ["4"]}</t>
   </si>
 </sst>
 </file>
@@ -346,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -412,6 +410,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -454,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -486,6 +490,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9D2251-14B4-1F49-81A1-F886FE8AA11B}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -879,7 +884,7 @@
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
     <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -925,8 +930,8 @@
       <c r="F2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>97</v>
+      <c r="G2" s="21" t="s">
+        <v>94</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>87</v>
@@ -948,8 +953,8 @@
       <c r="F3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>94</v>
+      <c r="G3" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>88</v>
@@ -971,8 +976,8 @@
       <c r="F4" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>93</v>
+      <c r="G4" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>89</v>
@@ -994,8 +999,8 @@
       <c r="F5" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>95</v>
+      <c r="G5" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>90</v>
@@ -1017,8 +1022,8 @@
       <c r="F6" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>93</v>
+      <c r="G6" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>91</v>
@@ -1040,8 +1045,8 @@
       <c r="F7" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>95</v>
+      <c r="G7" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>92</v>
@@ -1064,7 +1069,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
In 1112 - Fix counts (#530)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F471E059-E9F2-6449-9C1B-619B6455E888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E2BC4-31FE-8342-8452-9DB36BF6598B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -24,14 +24,12 @@
     <sheet name="client_nodebtchase_warnings" sheetId="7" r:id="rId9"/>
     <sheet name="person_warning" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -324,19 +322,19 @@
     <t>Deputy No, VWM</t>
   </si>
   <si>
-    <t>c_sim = not null</t>
-  </si>
-  <si>
-    <t>c_saar_check = not null</t>
-  </si>
-  <si>
-    <t>c_vwm = not null</t>
-  </si>
-  <si>
     <t>c_pri = 1</t>
   </si>
   <si>
-    <t>c_debt_chase = not null</t>
+    <t>include_values = {"col": "Debt chase", "values": ["1"]}</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "SAAR Check", "values": ["Y"]}</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "SIM", "values": ["3"]}</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "VWM", "values": ["4"]}</t>
   </si>
 </sst>
 </file>
@@ -346,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -412,6 +410,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -454,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -486,6 +490,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9D2251-14B4-1F49-81A1-F886FE8AA11B}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -879,7 +884,7 @@
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
     <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -925,8 +930,8 @@
       <c r="F2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>97</v>
+      <c r="G2" s="21" t="s">
+        <v>94</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>87</v>
@@ -948,8 +953,8 @@
       <c r="F3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>94</v>
+      <c r="G3" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>88</v>
@@ -971,8 +976,8 @@
       <c r="F4" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>93</v>
+      <c r="G4" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>89</v>
@@ -994,8 +999,8 @@
       <c r="F5" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>95</v>
+      <c r="G5" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>90</v>
@@ -1017,8 +1022,8 @@
       <c r="F6" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>93</v>
+      <c r="G6" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>91</v>
@@ -1040,8 +1045,8 @@
       <c r="F7" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>95</v>
+      <c r="G7" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>92</v>
@@ -1064,7 +1069,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>85</v>

</xml_diff>